<commit_message>
Premier probleme de SEO fixé, légère optimisation accessibilité (visuel)
</commit_message>
<xml_diff>
--- a/rapports/Analyse_SEO_et_accessibilité.xlsx
+++ b/rapports/Analyse_SEO_et_accessibilité.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\Starting website\rapports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2032C7C0-5FE4-4377-B8D4-23998CD8DF44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F07369-2DB3-4A2C-A65A-4B40B7592D32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="5850" windowHeight="7940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>Categorie</t>
   </si>
@@ -65,6 +65,96 @@
   </si>
   <si>
     <t>Corriger les erreurs W3C</t>
+  </si>
+  <si>
+    <t>Compression image</t>
+  </si>
+  <si>
+    <t>Vérifier que la taille de l'image initial soit adapter a l'image souhaité</t>
+  </si>
+  <si>
+    <t>Résuolution d'image trop élévée donc ralentissement du chargement du site</t>
+  </si>
+  <si>
+    <t>Vérifier son code sur GTMetrix</t>
+  </si>
+  <si>
+    <t>Code JS</t>
+  </si>
+  <si>
+    <t>Les espâces dans le code JS ralenti l'execution du code</t>
+  </si>
+  <si>
+    <t>Compresser (minify) son code avec GTMetrix</t>
+  </si>
+  <si>
+    <t>Accessibilité</t>
+  </si>
+  <si>
+    <t>Contraste de couleur</t>
+  </si>
+  <si>
+    <t>Probleme de lien</t>
+  </si>
+  <si>
+    <t>Verifier son code sur Wave</t>
+  </si>
+  <si>
+    <t>Lien sans texte/Lien avec destination pas coherente...</t>
+  </si>
+  <si>
+    <t>Directement mettre en place le lien de destination</t>
+  </si>
+  <si>
+    <t>Tres faible contraste entre le texte et son background</t>
+  </si>
+  <si>
+    <t>Pensez a tous les utilisateurs lors de la conception</t>
+  </si>
+  <si>
+    <t>Appliquer les standards de contraste</t>
+  </si>
+  <si>
+    <t>SEO &amp; Accessibilité</t>
+  </si>
+  <si>
+    <t>Mauvaise balise html</t>
+  </si>
+  <si>
+    <t>Bien identifer les parties du site avant de le construire</t>
+  </si>
+  <si>
+    <t>Il n'y a que des balises &lt;div&gt; dans le code html</t>
+  </si>
+  <si>
+    <t>Faire une maquette du site et identifier les balises</t>
+  </si>
+  <si>
+    <t>Visuel</t>
+  </si>
+  <si>
+    <t>Tester son site sur differents appareils</t>
+  </si>
+  <si>
+    <t>Plusieurs probleme d'affichage sur differentes tailles d'écran</t>
+  </si>
+  <si>
+    <t>Bien travailler son responsive</t>
+  </si>
+  <si>
+    <t>Pas de fichier sitemap</t>
+  </si>
+  <si>
+    <t>Vérifier son code sur des outils SEO</t>
+  </si>
+  <si>
+    <t>Pas de fichier sitemap.xml pour optimiser l'interaction avec les bots</t>
+  </si>
+  <si>
+    <t>Mettre un fichier sitemap.xml</t>
+  </si>
+  <si>
+    <t>neilpatel.com</t>
   </si>
 </sst>
 </file>
@@ -352,15 +442,15 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.23046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="21.69140625" customWidth="1"/>
-    <col min="3" max="3" width="31.4609375" customWidth="1"/>
-    <col min="4" max="4" width="43.3046875" customWidth="1"/>
+    <col min="3" max="3" width="40.765625" customWidth="1"/>
+    <col min="4" max="4" width="53.53515625" customWidth="1"/>
     <col min="5" max="5" width="43.765625" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="26" width="10.53515625" customWidth="1"/>
@@ -413,7 +503,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -430,7 +520,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -445,14 +535,130 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
avancement rapport + Optimisation SEO + Optimisation responsiv
</commit_message>
<xml_diff>
--- a/rapports/Analyse_SEO_et_accessibilité.xlsx
+++ b/rapports/Analyse_SEO_et_accessibilité.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\Starting website\rapports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F07369-2DB3-4A2C-A65A-4B40B7592D32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4599E8A1-DDBF-4599-A202-6BB2970D9AA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="5850" windowHeight="7940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>Categorie</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Vérifier que la taille de l'image initial soit adapter a l'image souhaité</t>
   </si>
   <si>
-    <t>Résuolution d'image trop élévée donc ralentissement du chargement du site</t>
-  </si>
-  <si>
     <t>Vérifier son code sur GTMetrix</t>
   </si>
   <si>
@@ -155,6 +152,21 @@
   </si>
   <si>
     <t>neilpatel.com</t>
+  </si>
+  <si>
+    <t>Résolution d'image trop élévée donc ralentissement du chargement du site</t>
+  </si>
+  <si>
+    <t>Pas de meta description</t>
+  </si>
+  <si>
+    <t>Mettre une meta description pour le référencement</t>
+  </si>
+  <si>
+    <t>Sans meta description, le bot google sera moins efficace pour repérer les mots clés</t>
+  </si>
+  <si>
+    <t>Chercher les bons mots clés en rapport avec votre site qu'un utilisateur va taper pour le trouver et en placer dans cette description</t>
   </si>
 </sst>
 </file>
@@ -441,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.23046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -503,7 +515,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -520,7 +532,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -537,16 +549,16 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -554,84 +566,84 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
       <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
         <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -639,24 +651,39 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>42</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>43</v>
-      </c>
-      <c r="F11" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1649,6 +1676,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Optimisation Acessibilité + Responsive
</commit_message>
<xml_diff>
--- a/rapports/Analyse_SEO_et_accessibilité.xlsx
+++ b/rapports/Analyse_SEO_et_accessibilité.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\Starting website\rapports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5055CF62-5666-46D8-91F1-3BE74B5DCEF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904A5B9A-0D66-4CED-874C-0DE2E760CE58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="5850" windowHeight="7940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>Categorie</t>
   </si>
@@ -170,6 +170,18 @@
   </si>
   <si>
     <t>neilpatel.com et xml-sitemaps.com</t>
+  </si>
+  <si>
+    <t>Image a la place du texte</t>
+  </si>
+  <si>
+    <t>Une image a la place d'un texte, pas responsive, pas optimisé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réécrire le texte </t>
+  </si>
+  <si>
+    <t>Utiliser des paragraphes pour faire des citations</t>
   </si>
 </sst>
 </file>
@@ -456,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.23046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -689,7 +701,23 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Problème de contraste réglé sur la totalité du site
</commit_message>
<xml_diff>
--- a/rapports/Analyse_SEO_et_accessibilité.xlsx
+++ b/rapports/Analyse_SEO_et_accessibilité.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\Starting website\rapports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904A5B9A-0D66-4CED-874C-0DE2E760CE58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AA6E5A-9CD2-46ED-8C1F-C313324AD39B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="5850" windowHeight="7940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>Categorie</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>Utiliser des paragraphes pour faire des citations</t>
+  </si>
+  <si>
+    <t>app.contrast-finder.org</t>
   </si>
 </sst>
 </file>
@@ -468,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.23046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -608,6 +611,9 @@
       </c>
       <c r="E7" t="s">
         <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>